<commit_message>
starting to add last parts
</commit_message>
<xml_diff>
--- a/doc/thesis/pictures/resultate/loesung2/variante0/resultate_mit_byte.xlsx
+++ b/doc/thesis/pictures/resultate/loesung2/variante0/resultate_mit_byte.xlsx
@@ -669,13 +669,13 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="268441136"/>
-        <c:axId val="268444272"/>
+        <c:axId val="267044160"/>
+        <c:axId val="267045336"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="268441136"/>
+        <c:axId val="267044160"/>
         <c:scaling>
-          <c:logBase val="10"/>
+          <c:logBase val="2"/>
           <c:orientation val="minMax"/>
           <c:min val="50"/>
         </c:scaling>
@@ -797,13 +797,12 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="268444272"/>
+        <c:crossAx val="267045336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
-        <c:majorUnit val="10"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="268444272"/>
+        <c:axId val="267045336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -916,7 +915,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="268441136"/>
+        <c:crossAx val="267044160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:dispUnits>

</xml_diff>